<commit_message>
General syncing of dev to prod
</commit_message>
<xml_diff>
--- a/workbooks/ClientWorkGrid.xlsx
+++ b/workbooks/ClientWorkGrid.xlsx
@@ -38,15 +38,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>&lt;clientName&gt;</t>
-  </si>
-  <si>
-    <t>&lt;csm&gt;</t>
-  </si>
-  <si>
-    <t>Recieved Initial Workflow Request</t>
-  </si>
-  <si>
     <t>Courses</t>
   </si>
   <si>
@@ -54,6 +45,15 @@
   </si>
   <si>
     <t>Other</t>
+  </si>
+  <si>
+    <t>&lt;csm&gt;</t>
+  </si>
+  <si>
+    <t>&lt;clientCode&gt;</t>
+  </si>
+  <si>
+    <t>Received initial request for</t>
   </si>
 </sst>
 </file>
@@ -631,6 +631,54 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -647,54 +695,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -748,7 +748,7 @@
             <a:xfrm>
               <a:off x="895350" y="704850"/>
               <a:ext cx="2419350" cy="133350"/>
-              <a:chOff x="952500" y="800100"/>
+              <a:chOff x="952500" y="800098"/>
               <a:chExt cx="2419350" cy="171450"/>
             </a:xfrm>
           </xdr:grpSpPr>
@@ -765,7 +765,7 @@
             </xdr:nvSpPr>
             <xdr:spPr bwMode="auto">
               <a:xfrm>
-                <a:off x="952500" y="800102"/>
+                <a:off x="952500" y="800103"/>
                 <a:ext cx="1238250" cy="163657"/>
               </a:xfrm>
               <a:prstGeom prst="rect">
@@ -829,7 +829,7 @@
             </xdr:nvSpPr>
             <xdr:spPr bwMode="auto">
               <a:xfrm>
-                <a:off x="2343150" y="800100"/>
+                <a:off x="2343150" y="800098"/>
                 <a:ext cx="1028700" cy="171450"/>
               </a:xfrm>
               <a:prstGeom prst="rect">
@@ -1180,44 +1180,44 @@
   <dimension ref="A3:I31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:C9"/>
+      <selection activeCell="B6" sqref="B6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="11.5703125" style="6" customWidth="1"/>
     <col min="3" max="3" width="59.7109375" customWidth="1"/>
-    <col min="4" max="4" width="3" style="40" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3" style="40" customWidth="1"/>
-    <col min="6" max="6" width="3" style="40" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3" style="34" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3" style="34" customWidth="1"/>
+    <col min="6" max="6" width="3" style="34" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="3" style="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="2.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:9" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
-        <v>6</v>
+      <c r="A3" s="45" t="s">
+        <v>8</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="28" t="s">
-        <v>5</v>
+      <c r="B3" s="45"/>
+      <c r="C3" s="44" t="s">
+        <v>9</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
     </row>
     <row r="4" spans="1:9" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="30" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
       <c r="I4" s="13"/>
@@ -1230,16 +1230,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="26"/>
-      <c r="D5" s="37" t="s">
-        <v>8</v>
+      <c r="D5" s="31" t="s">
+        <v>5</v>
       </c>
-      <c r="E5" s="38" t="s">
-        <v>9</v>
+      <c r="E5" s="32" t="s">
+        <v>6</v>
       </c>
-      <c r="F5" s="39" t="s">
-        <v>10</v>
+      <c r="F5" s="33" t="s">
+        <v>7</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="29" t="s">
         <v>3</v>
       </c>
       <c r="H5" s="14" t="s">
@@ -1252,257 +1252,257 @@
     <row r="6" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <f ca="1">TODAY()</f>
-        <v>42772</v>
+        <v>42814</v>
       </c>
-      <c r="B6" s="30" t="s">
-        <v>7</v>
+      <c r="B6" s="46" t="s">
+        <v>10</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="34"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="28"/>
       <c r="H6" s="16"/>
       <c r="I6" s="17"/>
     </row>
     <row r="7" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="46"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="40"/>
       <c r="G7" s="18"/>
       <c r="H7" s="19"/>
       <c r="I7" s="20"/>
     </row>
     <row r="8" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="46"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="40"/>
       <c r="G8" s="18"/>
       <c r="H8" s="19"/>
       <c r="I8" s="20"/>
     </row>
     <row r="9" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="46"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="40"/>
       <c r="G9" s="18"/>
       <c r="H9" s="19"/>
       <c r="I9" s="20"/>
     </row>
     <row r="10" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="46"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="40"/>
       <c r="G10" s="18"/>
       <c r="H10" s="19"/>
       <c r="I10" s="20"/>
     </row>
     <row r="11" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="46"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="40"/>
       <c r="G11" s="18"/>
       <c r="H11" s="19"/>
       <c r="I11" s="20"/>
     </row>
     <row r="12" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="46"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="40"/>
       <c r="G12" s="18"/>
       <c r="H12" s="19"/>
       <c r="I12" s="20"/>
     </row>
     <row r="13" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="46"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="40"/>
       <c r="G13" s="18"/>
       <c r="H13" s="19"/>
       <c r="I13" s="20"/>
     </row>
     <row r="14" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="46"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="40"/>
       <c r="G14" s="18"/>
       <c r="H14" s="19"/>
       <c r="I14" s="20"/>
     </row>
     <row r="15" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="46"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="40"/>
       <c r="G15" s="18"/>
       <c r="H15" s="19"/>
       <c r="I15" s="20"/>
     </row>
     <row r="16" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="46"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="40"/>
       <c r="G16" s="18"/>
       <c r="H16" s="19"/>
       <c r="I16" s="20"/>
     </row>
     <row r="17" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="46"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="40"/>
       <c r="G17" s="18"/>
       <c r="H17" s="19"/>
       <c r="I17" s="20"/>
     </row>
     <row r="18" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="46"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="40"/>
       <c r="G18" s="18"/>
       <c r="H18" s="19"/>
       <c r="I18" s="20"/>
     </row>
     <row r="19" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="46"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="40"/>
       <c r="G19" s="18"/>
       <c r="H19" s="19"/>
       <c r="I19" s="20"/>
     </row>
     <row r="20" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="46"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="40"/>
       <c r="G20" s="18"/>
       <c r="H20" s="19"/>
       <c r="I20" s="20"/>
     </row>
     <row r="21" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
-      <c r="B21" s="32"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="46"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="40"/>
       <c r="G21" s="18"/>
       <c r="H21" s="19"/>
       <c r="I21" s="20"/>
     </row>
     <row r="22" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="46"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="40"/>
       <c r="G22" s="18"/>
       <c r="H22" s="19"/>
       <c r="I22" s="20"/>
     </row>
     <row r="23" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
-      <c r="B23" s="32"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="46"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="40"/>
       <c r="G23" s="18"/>
       <c r="H23" s="19"/>
       <c r="I23" s="20"/>
     </row>
     <row r="24" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="46"/>
+      <c r="B24" s="48"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="40"/>
       <c r="G24" s="18"/>
       <c r="H24" s="19"/>
       <c r="I24" s="20"/>
     </row>
     <row r="25" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
-      <c r="B25" s="32"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="46"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="40"/>
       <c r="G25" s="18"/>
       <c r="H25" s="19"/>
       <c r="I25" s="20"/>
     </row>
     <row r="26" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
-      <c r="B26" s="32"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="46"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="40"/>
       <c r="G26" s="18"/>
       <c r="H26" s="19"/>
       <c r="I26" s="20"/>
     </row>
     <row r="27" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
-      <c r="B27" s="32"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="46"/>
+      <c r="B27" s="48"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="40"/>
       <c r="G27" s="18"/>
       <c r="H27" s="19"/>
       <c r="I27" s="20"/>
     </row>
     <row r="28" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="46"/>
+      <c r="B28" s="48"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="40"/>
       <c r="G28" s="18"/>
       <c r="H28" s="19"/>
       <c r="I28" s="20"/>
@@ -1511,9 +1511,9 @@
       <c r="A29" s="8"/>
       <c r="B29" s="24"/>
       <c r="C29" s="10"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="46"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="40"/>
       <c r="G29" s="18"/>
       <c r="H29" s="19"/>
       <c r="I29" s="20"/>
@@ -1522,9 +1522,9 @@
       <c r="A30" s="9"/>
       <c r="B30" s="25"/>
       <c r="C30" s="11"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="49"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="43"/>
       <c r="G30" s="21"/>
       <c r="H30" s="22"/>
       <c r="I30" s="23"/>

</xml_diff>

<commit_message>
Modified the tracking columns
</commit_message>
<xml_diff>
--- a/workbooks/ClientWorkGrid.xlsx
+++ b/workbooks/ClientWorkGrid.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -30,21 +30,6 @@
   </si>
   <si>
     <t>Origin:</t>
-  </si>
-  <si>
-    <t>Task</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Courses</t>
-  </si>
-  <si>
-    <t>Programs</t>
-  </si>
-  <si>
-    <t>Other</t>
   </si>
   <si>
     <t>&lt;csm&gt;</t>
@@ -57,6 +42,15 @@
   </si>
   <si>
     <t>Waiting</t>
+  </si>
+  <si>
+    <t>Instance</t>
+  </si>
+  <si>
+    <t>Env</t>
+  </si>
+  <si>
+    <t>Req Source</t>
   </si>
 </sst>
 </file>
@@ -150,32 +144,29 @@
     </font>
     <font>
       <b/>
-      <sz val="8"/>
-      <color rgb="FF0070C0"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-      <scheme val="major"/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-      <scheme val="major"/>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FFFF0000"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-      <scheme val="major"/>
+      <sz val="9"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
+      <sz val="9"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -189,7 +180,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -338,97 +329,9 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="double">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="double">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="double">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="double">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="double">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="double">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="double">
-        <color auto="1"/>
-      </right>
-      <top style="double">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="hair">
         <color auto="1"/>
       </right>
@@ -550,8 +453,12 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -564,13 +471,58 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="hair">
-        <color indexed="64"/>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -579,7 +531,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -606,31 +558,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -639,22 +573,49 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -663,77 +624,41 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -786,7 +711,7 @@
             <a:xfrm>
               <a:off x="895350" y="704850"/>
               <a:ext cx="2419350" cy="133350"/>
-              <a:chOff x="952500" y="800097"/>
+              <a:chOff x="952500" y="800095"/>
               <a:chExt cx="2419350" cy="171450"/>
             </a:xfrm>
           </xdr:grpSpPr>
@@ -867,7 +792,7 @@
             </xdr:nvSpPr>
             <xdr:spPr bwMode="auto">
               <a:xfrm>
-                <a:off x="2343150" y="800097"/>
+                <a:off x="2343150" y="800095"/>
                 <a:ext cx="1028700" cy="171450"/>
               </a:xfrm>
               <a:prstGeom prst="rect">
@@ -1215,414 +1140,323 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A3:J31"/>
+  <dimension ref="A3:G31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="41" customWidth="1"/>
-    <col min="3" max="3" width="59.7109375" style="42" customWidth="1"/>
-    <col min="4" max="4" width="3" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="3" style="20" customWidth="1"/>
-    <col min="7" max="7" width="3" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="3" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="25" customWidth="1"/>
+    <col min="3" max="3" width="66.42578125" style="26" customWidth="1"/>
+    <col min="4" max="4" width="3" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3" style="14" customWidth="1"/>
+    <col min="6" max="7" width="3" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
-        <v>8</v>
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="31" t="s">
+        <v>3</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="27" t="s">
-        <v>9</v>
+      <c r="B3" s="31"/>
+      <c r="C3" s="30" t="s">
+        <v>4</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-    </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+    </row>
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="9"/>
-    </row>
-    <row r="5" spans="1:10" s="2" customFormat="1" ht="45" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="39"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="9"/>
+    </row>
+    <row r="5" spans="1:7" s="2" customFormat="1" ht="52.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="49" t="s">
-        <v>11</v>
+      <c r="C5" s="20"/>
+      <c r="D5" s="40" t="s">
+        <v>6</v>
       </c>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="43" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="I5" s="47" t="s">
-        <v>4</v>
-      </c>
-      <c r="J5" s="48" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="11"/>
-    </row>
-    <row r="7" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="33"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="36"/>
+    </row>
+    <row r="7" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="14"/>
-    </row>
-    <row r="8" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="34"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="37"/>
+    </row>
+    <row r="8" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="14"/>
-    </row>
-    <row r="9" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="34"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="37"/>
+    </row>
+    <row r="9" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="14"/>
-    </row>
-    <row r="10" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="34"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="37"/>
+    </row>
+    <row r="10" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="14"/>
-    </row>
-    <row r="11" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="34"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="37"/>
+    </row>
+    <row r="11" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="14"/>
-    </row>
-    <row r="12" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="34"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="37"/>
+    </row>
+    <row r="12" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="14"/>
-    </row>
-    <row r="13" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="34"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="37"/>
+    </row>
+    <row r="13" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="14"/>
-    </row>
-    <row r="14" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="34"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="37"/>
+    </row>
+    <row r="14" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="14"/>
-    </row>
-    <row r="15" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="34"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="37"/>
+    </row>
+    <row r="15" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="14"/>
-    </row>
-    <row r="16" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="34"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="37"/>
+    </row>
+    <row r="16" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="14"/>
-    </row>
-    <row r="17" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="34"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="37"/>
+    </row>
+    <row r="17" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="14"/>
-    </row>
-    <row r="18" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="34"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="37"/>
+    </row>
+    <row r="18" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="14"/>
-    </row>
-    <row r="19" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="34"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="37"/>
+    </row>
+    <row r="19" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="14"/>
-    </row>
-    <row r="20" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="34"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="37"/>
+    </row>
+    <row r="20" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="14"/>
-    </row>
-    <row r="21" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="34"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="37"/>
+    </row>
+    <row r="21" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
-      <c r="B21" s="35"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="14"/>
-    </row>
-    <row r="22" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="34"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="37"/>
+    </row>
+    <row r="22" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
-      <c r="B22" s="35"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="14"/>
-    </row>
-    <row r="23" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="34"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="37"/>
+    </row>
+    <row r="23" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="14"/>
-    </row>
-    <row r="24" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="34"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="37"/>
+    </row>
+    <row r="24" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="51"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="14"/>
-    </row>
-    <row r="25" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="34"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="37"/>
+    </row>
+    <row r="25" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
-      <c r="B25" s="35"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="51"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="14"/>
-    </row>
-    <row r="26" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="34"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="37"/>
+    </row>
+    <row r="26" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="14"/>
-    </row>
-    <row r="27" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="34"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="37"/>
+    </row>
+    <row r="27" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
-      <c r="B27" s="35"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="51"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="14"/>
-    </row>
-    <row r="28" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="34"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="37"/>
+    </row>
+    <row r="28" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
-      <c r="B28" s="35"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="14"/>
-    </row>
-    <row r="29" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="34"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="37"/>
+    </row>
+    <row r="29" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
-      <c r="B29" s="37"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="14"/>
-    </row>
-    <row r="30" spans="1:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="21"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="37"/>
+    </row>
+    <row r="30" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
-      <c r="B30" s="39"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="17"/>
-    </row>
-    <row r="31" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="38"/>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.25" bottom="0.25" header="0" footer="0"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Added new columns for instance
</commit_message>
<xml_diff>
--- a/workbooks/ClientWorkGrid.xlsx
+++ b/workbooks/ClientWorkGrid.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\saugus\dscudiero\tools\workbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\tools\workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -44,13 +44,19 @@
     <t>Waiting</t>
   </si>
   <si>
-    <t>Instance</t>
-  </si>
-  <si>
     <t>Env</t>
   </si>
   <si>
     <t>Req Source</t>
+  </si>
+  <si>
+    <t>Courses</t>
+  </si>
+  <si>
+    <t>Programs</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -158,7 +164,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -225,9 +231,65 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top style="double">
         <color auto="1"/>
@@ -238,9 +300,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
+      <left/>
       <right/>
       <top style="hair">
         <color auto="1"/>
@@ -251,9 +311,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
+      <left/>
       <right/>
       <top style="hair">
         <color auto="1"/>
@@ -264,12 +322,83 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="hair">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
       <top style="hair">
         <color auto="1"/>
       </top>
@@ -280,23 +409,66 @@
     </border>
     <border>
       <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
       </left>
       <right style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="hair">
         <color auto="1"/>
       </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
       <bottom style="double">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -307,10 +479,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
         <color auto="1"/>
       </right>
       <top style="double">
@@ -322,79 +494,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="double">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="double">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="double">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -407,9 +509,11 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="hair">
         <color auto="1"/>
@@ -420,81 +524,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="double">
-        <color auto="1"/>
-      </right>
-      <top style="double">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="double">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="double">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="double">
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
         <color auto="1"/>
       </right>
       <top style="hair">
@@ -509,7 +542,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -536,22 +569,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -563,11 +587,50 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -575,64 +638,43 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -666,13 +708,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor>
         <xdr:from>
-          <xdr:col>1</xdr:col>
+          <xdr:col>4</xdr:col>
           <xdr:colOff>66675</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>2</xdr:col>
+          <xdr:col>5</xdr:col>
           <xdr:colOff>1657350</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
@@ -684,9 +726,9 @@
           </xdr:nvGrpSpPr>
           <xdr:grpSpPr>
             <a:xfrm>
-              <a:off x="895350" y="704850"/>
+              <a:off x="1390650" y="704850"/>
               <a:ext cx="2419350" cy="133350"/>
-              <a:chOff x="952500" y="800094"/>
+              <a:chOff x="952500" y="800093"/>
               <a:chExt cx="2419350" cy="171450"/>
             </a:xfrm>
           </xdr:grpSpPr>
@@ -767,7 +809,7 @@
             </xdr:nvSpPr>
             <xdr:spPr bwMode="auto">
               <a:xfrm>
-                <a:off x="2343150" y="800094"/>
+                <a:off x="2343150" y="800093"/>
                 <a:ext cx="1028700" cy="171450"/>
               </a:xfrm>
               <a:prstGeom prst="rect">
@@ -1115,323 +1157,384 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A3:G31"/>
+  <dimension ref="A3:I31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:C11"/>
+    <sheetView showGridLines="0" tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="66.42578125" style="17" customWidth="1"/>
-    <col min="4" max="4" width="3" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3" style="25" customWidth="1"/>
-    <col min="6" max="7" width="3" style="26" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.28515625" customWidth="1"/>
+    <col min="2" max="3" width="2.28515625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="2.42578125" style="16" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="63.42578125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="3" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="3" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+    <row r="3" spans="1:9" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="21" t="s">
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-    </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+    </row>
+    <row r="4" spans="1:9" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-    </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" ht="48.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+    </row>
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="48.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="27" t="s">
+      <c r="F5" s="10"/>
+      <c r="G5" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="H5" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="30" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="22"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="32"/>
       <c r="F6" s="33"/>
-      <c r="G6" s="34"/>
-    </row>
-    <row r="7" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="22"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="24"/>
+    </row>
+    <row r="7" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="38"/>
-    </row>
-    <row r="8" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="25"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="27"/>
+    </row>
+    <row r="8" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="38"/>
-    </row>
-    <row r="9" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="25"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="27"/>
+    </row>
+    <row r="9" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="38"/>
-    </row>
-    <row r="10" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="25"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="27"/>
+    </row>
+    <row r="10" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="38"/>
-    </row>
-    <row r="11" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="25"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="27"/>
+    </row>
+    <row r="11" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="38"/>
-    </row>
-    <row r="12" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="25"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="27"/>
+    </row>
+    <row r="12" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="38"/>
-    </row>
-    <row r="13" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="25"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="27"/>
+    </row>
+    <row r="13" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="38"/>
-    </row>
-    <row r="14" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="25"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="27"/>
+    </row>
+    <row r="14" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="38"/>
-    </row>
-    <row r="15" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="25"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="27"/>
+    </row>
+    <row r="15" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="38"/>
-    </row>
-    <row r="16" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="25"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="27"/>
+    </row>
+    <row r="16" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="38"/>
-    </row>
-    <row r="17" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="25"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="27"/>
+    </row>
+    <row r="17" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="38"/>
-    </row>
-    <row r="18" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="25"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="27"/>
+    </row>
+    <row r="18" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="38"/>
-    </row>
-    <row r="19" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="25"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="27"/>
+    </row>
+    <row r="19" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="38"/>
-    </row>
-    <row r="20" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="25"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="27"/>
+    </row>
+    <row r="20" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="38"/>
-    </row>
-    <row r="21" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="25"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="27"/>
+    </row>
+    <row r="21" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="38"/>
-    </row>
-    <row r="22" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="25"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="27"/>
+    </row>
+    <row r="22" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="38"/>
-    </row>
-    <row r="23" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="25"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="27"/>
+    </row>
+    <row r="23" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="38"/>
-    </row>
-    <row r="24" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="25"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="27"/>
+    </row>
+    <row r="24" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="38"/>
-    </row>
-    <row r="25" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="25"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="27"/>
+    </row>
+    <row r="25" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="38"/>
-    </row>
-    <row r="26" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="25"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="27"/>
+    </row>
+    <row r="26" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="38"/>
-    </row>
-    <row r="27" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="25"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="27"/>
+    </row>
+    <row r="27" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="38"/>
-    </row>
-    <row r="28" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="25"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="27"/>
+    </row>
+    <row r="28" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="38"/>
-    </row>
-    <row r="29" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="25"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="27"/>
+    </row>
+    <row r="29" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="38"/>
-    </row>
-    <row r="30" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="25"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="27"/>
+    </row>
+    <row r="30" spans="1:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="42"/>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="30"/>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.25" bottom="0.25" header="0" footer="0"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -1446,13 +1549,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>1</xdr:col>
+                    <xdr:col>4</xdr:col>
                     <xdr:colOff>66675</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>2</xdr:col>
+                    <xdr:col>5</xdr:col>
                     <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>123825</xdr:rowOff>
@@ -1468,13 +1571,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>2</xdr:col>
+                    <xdr:col>5</xdr:col>
                     <xdr:colOff>628650</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>2</xdr:col>
+                    <xdr:col>5</xdr:col>
                     <xdr:colOff>1657350</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>133350</xdr:rowOff>

</xml_diff>

<commit_message>
Updates to enable advanced Help processing
</commit_message>
<xml_diff>
--- a/workbooks/ClientWorkGrid.xlsx
+++ b/workbooks/ClientWorkGrid.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -30,15 +30,6 @@
   </si>
   <si>
     <t>Origin:</t>
-  </si>
-  <si>
-    <t>&lt;csm&gt;</t>
-  </si>
-  <si>
-    <t>&lt;clientCode&gt;</t>
-  </si>
-  <si>
-    <t>Received initial request for</t>
   </si>
   <si>
     <t>Waiting</t>
@@ -57,6 +48,12 @@
   </si>
   <si>
     <t>Other</t>
+  </si>
+  <si>
+    <t>&lt;CSM&gt;</t>
+  </si>
+  <si>
+    <t>&lt;clientCode&gt;</t>
   </si>
 </sst>
 </file>
@@ -632,50 +629,50 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -728,7 +725,7 @@
             <a:xfrm>
               <a:off x="1390650" y="704850"/>
               <a:ext cx="2419350" cy="133350"/>
-              <a:chOff x="952500" y="800093"/>
+              <a:chOff x="952500" y="800090"/>
               <a:chExt cx="2419350" cy="171450"/>
             </a:xfrm>
           </xdr:grpSpPr>
@@ -809,7 +806,7 @@
             </xdr:nvSpPr>
             <xdr:spPr bwMode="auto">
               <a:xfrm>
-                <a:off x="2343150" y="800093"/>
+                <a:off x="2343150" y="800090"/>
                 <a:ext cx="1028700" cy="171450"/>
               </a:xfrm>
               <a:prstGeom prst="rect">
@@ -1160,7 +1157,7 @@
   <dimension ref="A3:I31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="E11" sqref="E11:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1176,19 +1173,19 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:9" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
-        <v>3</v>
+      <c r="A3" s="41" t="s">
+        <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="31" t="s">
-        <v>4</v>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="40" t="s">
+        <v>10</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
     </row>
     <row r="4" spans="1:9" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
@@ -1208,37 +1205,35 @@
         <v>0</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
-      <c r="D5" s="42" t="s">
-        <v>11</v>
+      <c r="D5" s="36" t="s">
+        <v>8</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="18" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="22"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="33"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="43"/>
       <c r="G6" s="22"/>
       <c r="H6" s="23"/>
       <c r="I6" s="24"/>
@@ -1246,10 +1241,10 @@
     <row r="7" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="25"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="34"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="45"/>
       <c r="G7" s="25"/>
       <c r="H7" s="26"/>
       <c r="I7" s="27"/>
@@ -1257,10 +1252,10 @@
     <row r="8" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="25"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="34"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="45"/>
       <c r="G8" s="25"/>
       <c r="H8" s="26"/>
       <c r="I8" s="27"/>
@@ -1268,10 +1263,10 @@
     <row r="9" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="25"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="34"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="45"/>
       <c r="G9" s="25"/>
       <c r="H9" s="26"/>
       <c r="I9" s="27"/>
@@ -1279,10 +1274,10 @@
     <row r="10" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="25"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="34"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="45"/>
       <c r="G10" s="25"/>
       <c r="H10" s="26"/>
       <c r="I10" s="27"/>
@@ -1290,10 +1285,10 @@
     <row r="11" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="25"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="34"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="45"/>
       <c r="G11" s="25"/>
       <c r="H11" s="26"/>
       <c r="I11" s="27"/>
@@ -1301,10 +1296,10 @@
     <row r="12" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="25"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="34"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="45"/>
       <c r="G12" s="25"/>
       <c r="H12" s="26"/>
       <c r="I12" s="27"/>
@@ -1312,10 +1307,10 @@
     <row r="13" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="25"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="34"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="45"/>
       <c r="G13" s="25"/>
       <c r="H13" s="26"/>
       <c r="I13" s="27"/>
@@ -1323,10 +1318,10 @@
     <row r="14" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="25"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="34"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="45"/>
       <c r="G14" s="25"/>
       <c r="H14" s="26"/>
       <c r="I14" s="27"/>
@@ -1334,10 +1329,10 @@
     <row r="15" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="25"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="34"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="45"/>
       <c r="G15" s="25"/>
       <c r="H15" s="26"/>
       <c r="I15" s="27"/>
@@ -1345,10 +1340,10 @@
     <row r="16" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="25"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="34"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="45"/>
       <c r="G16" s="25"/>
       <c r="H16" s="26"/>
       <c r="I16" s="27"/>
@@ -1356,10 +1351,10 @@
     <row r="17" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="25"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="34"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="45"/>
       <c r="G17" s="25"/>
       <c r="H17" s="26"/>
       <c r="I17" s="27"/>
@@ -1367,10 +1362,10 @@
     <row r="18" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="25"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="34"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="45"/>
       <c r="G18" s="25"/>
       <c r="H18" s="26"/>
       <c r="I18" s="27"/>
@@ -1378,10 +1373,10 @@
     <row r="19" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="25"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="34"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="45"/>
       <c r="G19" s="25"/>
       <c r="H19" s="26"/>
       <c r="I19" s="27"/>
@@ -1389,10 +1384,10 @@
     <row r="20" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="25"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="34"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="45"/>
       <c r="G20" s="25"/>
       <c r="H20" s="26"/>
       <c r="I20" s="27"/>
@@ -1400,10 +1395,10 @@
     <row r="21" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="25"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="34"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="45"/>
       <c r="G21" s="25"/>
       <c r="H21" s="26"/>
       <c r="I21" s="27"/>
@@ -1411,10 +1406,10 @@
     <row r="22" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="25"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="34"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="45"/>
       <c r="G22" s="25"/>
       <c r="H22" s="26"/>
       <c r="I22" s="27"/>
@@ -1422,10 +1417,10 @@
     <row r="23" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="25"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="34"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="45"/>
       <c r="G23" s="25"/>
       <c r="H23" s="26"/>
       <c r="I23" s="27"/>
@@ -1433,10 +1428,10 @@
     <row r="24" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="25"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="34"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="45"/>
       <c r="G24" s="25"/>
       <c r="H24" s="26"/>
       <c r="I24" s="27"/>
@@ -1444,10 +1439,10 @@
     <row r="25" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="25"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="34"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="45"/>
       <c r="G25" s="25"/>
       <c r="H25" s="26"/>
       <c r="I25" s="27"/>
@@ -1455,10 +1450,10 @@
     <row r="26" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="25"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="34"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="45"/>
       <c r="G26" s="25"/>
       <c r="H26" s="26"/>
       <c r="I26" s="27"/>
@@ -1466,10 +1461,10 @@
     <row r="27" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="25"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="34"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="45"/>
       <c r="G27" s="25"/>
       <c r="H27" s="26"/>
       <c r="I27" s="27"/>
@@ -1477,10 +1472,10 @@
     <row r="28" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="25"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="34"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="45"/>
       <c r="G28" s="25"/>
       <c r="H28" s="26"/>
       <c r="I28" s="27"/>
@@ -1488,10 +1483,10 @@
     <row r="29" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="25"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="44"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="38"/>
       <c r="E29" s="11"/>
-      <c r="F29" s="38"/>
+      <c r="F29" s="34"/>
       <c r="G29" s="25"/>
       <c r="H29" s="26"/>
       <c r="I29" s="27"/>
@@ -1499,10 +1494,10 @@
     <row r="30" spans="1:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" s="28"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="45"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="39"/>
       <c r="E30" s="12"/>
-      <c r="F30" s="39"/>
+      <c r="F30" s="35"/>
       <c r="G30" s="28"/>
       <c r="H30" s="29"/>
       <c r="I30" s="30"/>
@@ -1537,7 +1532,7 @@
     <mergeCell ref="E8:F8"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.25" bottom="0.25" header="0" footer="0"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">

</xml_diff>